<commit_message>
excel of paper complete
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\job\phd-project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\thesis_phd\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8B41119-D8E3-4FC0-A9F0-585A3575EAA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
   <si>
     <t>Optimization parameters</t>
   </si>
@@ -134,21 +135,43 @@
     <t xml:space="preserve">maximize the QoS (formula based on rate, delay and probability of error) with the constraint of maximum power, min and max of rate </t>
   </si>
   <si>
-    <t>power, RB (find best policy for upper and lower level to assigne resources to slices )</t>
-  </si>
-  <si>
-    <t>the modified deep deterministic
-policy gradient (DDPG) and double deep-Q-network algorithm</t>
-  </si>
-  <si>
     <t>It has two timescale, and since that it has two level the upper and the lower level. the proposed method consists of an upper-level controller to ensure the QoS performance, which enforces loose control by
 performing adaptive slice configuration according to the longterm dynamics of service traffic. The lower-level controller is to improve SE of slices, by tightly scheduling radio resources to users at the small time-scale.</t>
+  </si>
+  <si>
+    <t>Intelligent Resource Scheduling for 5G Radio
+Access Network Slicing</t>
+  </si>
+  <si>
+    <t>propose an intelligent resource scheduling strategy (iRSS) for 5G RAN slicing. The main idea of iRSS is to exploit a collaborative learning framework which consists of deep learning (DL) in conjunction with Reinforcement Learning
+(RL)</t>
+  </si>
+  <si>
+    <t>DL is used to perform large time-scale resource
+allocation, while RL is used to perform on-line resource scheduling for tackling small time-scale network dynamics, including
+inaccurate prediction and unexpected network states</t>
+  </si>
+  <si>
+    <t>There is two problem. 1: resource allocation of large time scale 2. RA of small scale, In the first step, we want to minimize the mean-square-error (MSE) between the predicted value of assigned resource block  and the actual traffic volume of it. In the second step we want to minimize assigned RB subject to the thresholds we need</t>
+  </si>
+  <si>
+    <t>predicted value of assigned RB (pre assignement)- large time scale, fro small time scale-  number of slices and the time interval</t>
+  </si>
+  <si>
+    <t>LTSM -large time scale, Q-learning, classic AC and HRSA algorithms for small time scale</t>
+  </si>
+  <si>
+    <t xml:space="preserve">first the modified deep deterministic
+policy gradient (DDPG) for lower level and then the double deep-Q-network algorithm for upper level </t>
+  </si>
+  <si>
+    <t>power, RB (find best policy for upper and lower level to assigne resources to slices ) for lower level and the guarantee bit rate and maximum rate for upper level</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -625,11 +648,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A5:H11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" topLeftCell="B2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -754,19 +777,41 @@
         <v>28</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="G9" s="5" t="s">
         <v>26</v>
       </c>
       <c r="H9" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="16">
+        <v>5</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" s="5" t="s">
         <v>31</v>
       </c>
+      <c r="D10" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="H10" s="5" t="s">
+        <v>32</v>
+      </c>
     </row>
-    <row r="10" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="11" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="13"/>
     </row>

</xml_diff>